<commit_message>
Updated View.Table to bind to End Cell if specified. This is required for OneWayToSource tables, as their view models need to know how many objects to create.
Fixed StyleCop complaints.
</commit_message>
<xml_diff>
--- a/ExcelMvc/Sample.Views/Forbes2000.xlsx
+++ b/ExcelMvc/Sample.Views/Forbes2000.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="315" windowWidth="22590" windowHeight="9465"/>
+    <workbookView xWindow="45" yWindow="315" windowWidth="22590" windowHeight="9465" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Forbes" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="58">
   <si>
     <t xml:space="preserve">Company </t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Update Interval Seconds</t>
+  </si>
+  <si>
+    <t>End Cell</t>
   </si>
 </sst>
 </file>
@@ -3776,7 +3779,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AE2526"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
@@ -54641,16 +54644,16 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="37" style="7" customWidth="1"/>
     <col min="5" max="5" width="45" style="7" customWidth="1"/>
     <col min="6" max="6" width="72" style="7" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="7" customWidth="1"/>
@@ -55635,7 +55638,9 @@
       <c r="C76" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D76" s="10"/>
+      <c r="D76" s="70" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="str">
@@ -55648,7 +55653,10 @@
       <c r="C77" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D77" s="9"/>
+      <c r="D77" s="9" t="str">
+        <f ca="1">CELL("address",References!C11)</f>
+        <v>[Forbes2000.xlsx]References!$C$11</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">

</xml_diff>

<commit_message>
Removed ghost Excel session after real-time update (due to the getting/setting screen updating).  Not really sure what caused, but it is removed for now.
Need to re-visit why there is now a frightening amount of flickering when the sample app is started.
</commit_message>
<xml_diff>
--- a/ExcelMvc/Sample.Views/Forbes2000.xlsx
+++ b/ExcelMvc/Sample.Views/Forbes2000.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="315" windowWidth="22590" windowHeight="9465" activeTab="3"/>
+    <workbookView xWindow="45" yWindow="315" windowWidth="22590" windowHeight="9465"/>
   </bookViews>
   <sheets>
     <sheet name="Forbes" sheetId="1" r:id="rId1"/>
@@ -3779,7 +3779,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AE2526"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
@@ -54644,7 +54644,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>

</xml_diff>